<commit_message>
DatabaseHandler som erstatning for PgnReader
</commit_message>
<xml_diff>
--- a/second_game.xlsx
+++ b/second_game.xlsx
@@ -14,7 +14,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="118">
+  <si>
+    <t>Move Number</t>
+  </si>
+  <si>
+    <t>Player Name</t>
+  </si>
+  <si>
+    <t>Player Rating</t>
+  </si>
+  <si>
+    <t>Move</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
   <si>
     <t>Arasan 23.3 64-bit</t>
   </si>
@@ -359,8 +374,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -376,7 +399,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -384,12 +407,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,248 +725,251 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D121"/>
+  <dimension ref="A1:E122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1">
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
-        <v>2</v>
-      </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
         <v>3</v>
       </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>4</v>
-      </c>
       <c r="B7" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -933,27 +977,27 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -961,27 +1005,27 @@
         <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -989,27 +1033,27 @@
         <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D22" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D23" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1017,27 +1061,27 @@
         <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B25" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1045,27 +1089,27 @@
         <v>13</v>
       </c>
       <c r="B26" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B27" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1073,27 +1117,27 @@
         <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D28" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D29" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1101,27 +1145,27 @@
         <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D30" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1129,27 +1173,27 @@
         <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D32" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C33" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D33" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1157,27 +1201,27 @@
         <v>17</v>
       </c>
       <c r="B34" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B35" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D35" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1185,27 +1229,27 @@
         <v>18</v>
       </c>
       <c r="B36" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B37" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C37" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1213,27 +1257,27 @@
         <v>19</v>
       </c>
       <c r="B38" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B39" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C39" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D39" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1241,27 +1285,27 @@
         <v>20</v>
       </c>
       <c r="B40" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B41" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C41" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1269,27 +1313,27 @@
         <v>21</v>
       </c>
       <c r="B42" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B43" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C43" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D43" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1297,27 +1341,27 @@
         <v>22</v>
       </c>
       <c r="B44" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B45" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C45" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D45" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1325,27 +1369,27 @@
         <v>23</v>
       </c>
       <c r="B46" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C46" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D46" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B47" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C47" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D47" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1353,27 +1397,27 @@
         <v>24</v>
       </c>
       <c r="B48" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D48" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B49" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C49" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D49" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1381,27 +1425,27 @@
         <v>25</v>
       </c>
       <c r="B50" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D50" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B51" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C51" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D51" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1409,27 +1453,27 @@
         <v>26</v>
       </c>
       <c r="B52" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C52" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D52" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B53" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C53" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D53" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1437,27 +1481,27 @@
         <v>27</v>
       </c>
       <c r="B54" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D54" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B55" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C55" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D55" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1465,27 +1509,27 @@
         <v>28</v>
       </c>
       <c r="B56" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C56" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D56" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B57" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C57" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D57" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1493,27 +1537,27 @@
         <v>29</v>
       </c>
       <c r="B58" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C58" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D58" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B59" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C59" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D59" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1521,27 +1565,27 @@
         <v>30</v>
       </c>
       <c r="B60" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C60" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D60" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B61" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C61" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D61" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1549,27 +1593,27 @@
         <v>31</v>
       </c>
       <c r="B62" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C62" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D62" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B63" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C63" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D63" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1577,27 +1621,27 @@
         <v>32</v>
       </c>
       <c r="B64" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C64" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D64" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B65" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C65" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D65" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1605,27 +1649,27 @@
         <v>33</v>
       </c>
       <c r="B66" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C66" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D66" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B67" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C67" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D67" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1633,27 +1677,27 @@
         <v>34</v>
       </c>
       <c r="B68" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C68" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D68" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B69" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C69" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D69" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1661,27 +1705,27 @@
         <v>35</v>
       </c>
       <c r="B70" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C70" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D70" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B71" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C71" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D71" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1689,27 +1733,27 @@
         <v>36</v>
       </c>
       <c r="B72" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C72" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D72" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B73" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C73" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D73" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1717,27 +1761,27 @@
         <v>37</v>
       </c>
       <c r="B74" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C74" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D74" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B75" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C75" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D75" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1745,27 +1789,27 @@
         <v>38</v>
       </c>
       <c r="B76" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C76" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D76" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B77" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C77" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D77" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1773,27 +1817,27 @@
         <v>39</v>
       </c>
       <c r="B78" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C78" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D78" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B79" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C79" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D79" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1801,27 +1845,27 @@
         <v>40</v>
       </c>
       <c r="B80" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C80" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D80" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B81" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C81" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D81" t="s">
-        <v>79</v>
+        <v>32</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1829,27 +1873,27 @@
         <v>41</v>
       </c>
       <c r="B82" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C82" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D82" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B83" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C83" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D83" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1857,27 +1901,27 @@
         <v>42</v>
       </c>
       <c r="B84" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C84" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D84" t="s">
-        <v>4</v>
+        <v>86</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B85" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C85" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D85" t="s">
-        <v>82</v>
+        <v>9</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -1885,27 +1929,27 @@
         <v>43</v>
       </c>
       <c r="B86" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C86" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D86" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B87" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C87" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D87" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -1913,27 +1957,27 @@
         <v>44</v>
       </c>
       <c r="B88" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C88" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D88" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B89" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C89" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D89" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -1941,27 +1985,27 @@
         <v>45</v>
       </c>
       <c r="B90" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C90" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D90" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B91" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C91" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D91" t="s">
-        <v>87</v>
+        <v>44</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -1969,27 +2013,27 @@
         <v>46</v>
       </c>
       <c r="B92" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C92" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D92" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B93" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C93" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D93" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -1997,27 +2041,27 @@
         <v>47</v>
       </c>
       <c r="B94" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C94" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D94" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B95" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C95" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D95" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -2025,27 +2069,27 @@
         <v>48</v>
       </c>
       <c r="B96" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C96" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D96" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B97" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C97" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D97" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2053,27 +2097,27 @@
         <v>49</v>
       </c>
       <c r="B98" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C98" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D98" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B99" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C99" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D99" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -2081,27 +2125,27 @@
         <v>50</v>
       </c>
       <c r="B100" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C100" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D100" t="s">
-        <v>35</v>
+        <v>99</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B101" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C101" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D101" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -2109,27 +2153,27 @@
         <v>51</v>
       </c>
       <c r="B102" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C102" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D102" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="A103">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B103" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C103" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D103" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -2137,27 +2181,27 @@
         <v>52</v>
       </c>
       <c r="B104" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C104" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D104" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="105" spans="1:4">
       <c r="A105">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B105" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C105" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D105" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -2165,27 +2209,27 @@
         <v>53</v>
       </c>
       <c r="B106" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C106" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D106" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="107" spans="1:4">
       <c r="A107">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B107" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C107" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D107" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -2193,27 +2237,27 @@
         <v>54</v>
       </c>
       <c r="B108" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C108" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D108" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="109" spans="1:4">
       <c r="A109">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B109" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C109" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D109" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -2221,27 +2265,27 @@
         <v>55</v>
       </c>
       <c r="B110" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C110" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D110" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="111" spans="1:4">
       <c r="A111">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B111" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C111" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D111" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -2249,27 +2293,27 @@
         <v>56</v>
       </c>
       <c r="B112" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C112" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D112" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
     </row>
     <row r="113" spans="1:4">
       <c r="A113">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B113" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C113" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D113" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -2277,27 +2321,27 @@
         <v>57</v>
       </c>
       <c r="B114" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C114" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D114" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="115" spans="1:4">
       <c r="A115">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B115" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C115" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D115" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2305,27 +2349,27 @@
         <v>58</v>
       </c>
       <c r="B116" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C116" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D116" t="s">
-        <v>36</v>
+        <v>112</v>
       </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B117" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C117" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D117" t="s">
-        <v>108</v>
+        <v>41</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2333,27 +2377,27 @@
         <v>59</v>
       </c>
       <c r="B118" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C118" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D118" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B119" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C119" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D119" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -2361,27 +2405,41 @@
         <v>60</v>
       </c>
       <c r="B120" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C120" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D120" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="121" spans="1:4">
       <c r="A121">
+        <v>60</v>
+      </c>
+      <c r="B121" t="s">
+        <v>6</v>
+      </c>
+      <c r="C121" t="s">
+        <v>8</v>
+      </c>
+      <c r="D121" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122">
         <v>61</v>
       </c>
-      <c r="B121" t="s">
-        <v>0</v>
-      </c>
-      <c r="C121" t="s">
-        <v>2</v>
-      </c>
-      <c r="D121" t="s">
-        <v>112</v>
+      <c r="B122" t="s">
+        <v>5</v>
+      </c>
+      <c r="C122" t="s">
+        <v>7</v>
+      </c>
+      <c r="D122" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>